<commit_message>
Income Distribution table and plot
</commit_message>
<xml_diff>
--- a/Datasets/vjcortesa_Presurvey_questions overview.xlsx
+++ b/Datasets/vjcortesa_Presurvey_questions overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/jcortesarevalo_tudelft_nl/Documents/Documents/TUDelft/18_Game Data Analysis/R data analysis BEPs/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1116" documentId="11_F25DC773A252ABDACC10482FB9DB7A865ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{730CE2CA-4249-4F13-892C-91E7417FEBEB}"/>
+  <xr:revisionPtr revIDLastSave="1117" documentId="11_F25DC773A252ABDACC10482FB9DB7A865ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B5BEA3A-2316-43D3-997C-D36CCE88438C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -799,7 +799,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -826,9 +826,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1113,8 +1110,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1745,8 +1742,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2038,7 +2035,7 @@
         <v>2 = Eén keer in het afgelopen jaar</v>
       </c>
       <c r="H10" s="10" t="str">
-        <f t="shared" si="0"/>
+        <f>+H$9</f>
         <v>3 = Eén keer in de afgelopen zes maanden</v>
       </c>
       <c r="I10" s="10" t="str">
@@ -2110,7 +2107,7 @@
       <c r="C12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="1">
         <v>18</v>
       </c>
       <c r="E12" s="2">
@@ -2154,7 +2151,7 @@
       <c r="C13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="1">
         <v>19</v>
       </c>
       <c r="E13" s="2">
@@ -2198,7 +2195,7 @@
       <c r="C14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="1">
         <v>20</v>
       </c>
       <c r="E14" s="2">
@@ -2242,7 +2239,7 @@
       <c r="C15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="1">
         <v>21</v>
       </c>
       <c r="E15" s="2">
@@ -2286,7 +2283,7 @@
       <c r="C16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="1">
         <v>22</v>
       </c>
       <c r="E16" s="2">
@@ -2320,7 +2317,7 @@
       <c r="C17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="1">
         <v>23</v>
       </c>
       <c r="E17" s="2">
@@ -2853,8 +2850,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>